<commit_message>
correct fruit and vegetable value type
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHR.xlsx
+++ b/data_processing_elements-SHR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B07117-878E-4FBC-BFE1-31340E67B585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3090D410-CBAD-42B0-881F-6E013BCAB540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1541,7 +1541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1569,7 +1569,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1912,10 +1911,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M49" sqref="M49"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2571,7 @@
       <c r="M14" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="O14" s="8" t="s">
         <v>400</v>
       </c>
       <c r="P14" s="8" t="s">
@@ -3534,7 +3533,7 @@
         <v>145</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>146</v>
@@ -3610,7 +3609,7 @@
         <v>154</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>146</v>

</xml_diff>